<commit_message>
actualizacion libretas bancarias modal v11
</commit_message>
<xml_diff>
--- a/libretas_bancarias/subidas/prueba_cargado_2.xlsx
+++ b/libretas_bancarias/subidas/prueba_cargado_2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>LPZ</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>DEPOSITO A CUENTA ALVARO VALLEJO</t>
+  </si>
+  <si>
+    <t>PRUEBA TEST 2</t>
+  </si>
+  <si>
+    <t>PRUEBA TEST 4</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,6 +992,40 @@
         <v>11</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>44014</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1">
+        <v>41438426</v>
+      </c>
+      <c r="D30" s="3">
+        <v>100</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>44016</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1">
+        <v>41438426</v>
+      </c>
+      <c r="D31" s="3">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>